<commit_message>
flyers & api done, write left
</commit_message>
<xml_diff>
--- a/my_resources/qaautomation.xlsx
+++ b/my_resources/qaautomation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>Series Cast</t>
   </si>
@@ -211,12 +211,21 @@
   <si>
     <t>Condititions/Assertions</t>
   </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>https://emumba-test.herokuapp.com/</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +295,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -308,24 +331,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -334,11 +344,27 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -621,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,93 +661,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
+      <c r="A1" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>59</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>12345678</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>30012345678</v>
+        <v>28</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>12345678</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>30012345678</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B11" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -733,24 +772,25 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="11" style="4" customWidth="1"/>
-    <col min="3" max="4" width="36.5546875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="51.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="51.33203125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="15.21875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="11" style="3" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+    <row r="1" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="11" t="s">
         <v>57</v>
       </c>
@@ -758,150 +798,150 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="4">
         <v>201</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="10"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" ht="105.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="4">
         <v>200</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="4">
         <v>2</v>
       </c>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" ht="66" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:8" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <v>200</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="4">
         <v>2</v>
       </c>
-      <c r="H5" s="10"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -909,9 +949,10 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
implemented excel read/write functionality
</commit_message>
<xml_diff>
--- a/my_resources/qaautomation.xlsx
+++ b/my_resources/qaautomation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>Series Cast</t>
   </si>
@@ -219,6 +219,24 @@
   </si>
   <si>
     <t>https://emumba-test.herokuapp.com/</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>ghi</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>mno</t>
+  </si>
+  <si>
+    <t>pqr</t>
   </si>
 </sst>
 </file>
@@ -357,14 +375,14 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,7 +667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -697,7 +715,7 @@
       <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -791,12 +809,12 @@
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -972,11 +990,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -1164,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1177,28 +1195,41 @@
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-    </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>